<commit_message>
CET em funcao de numero de atomos (30 CRNs)
</commit_message>
<xml_diff>
--- a/num_atomos/crn512.xlsx
+++ b/num_atomos/crn512.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>CRN</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>crn_00027</t>
+  </si>
+  <si>
+    <t>crn_00028</t>
+  </si>
+  <si>
+    <t>crn_00029</t>
   </si>
 </sst>
 </file>
@@ -489,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1336,6 +1342,64 @@
         <v>236</v>
       </c>
     </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3473.204909</v>
+      </c>
+      <c r="C30" s="2">
+        <v>264.312233</v>
+      </c>
+      <c r="D30" s="2">
+        <v>-0.06714299999999999</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2.29813</v>
+      </c>
+      <c r="F30" s="2">
+        <v>53.125</v>
+      </c>
+      <c r="G30" s="2">
+        <v>6</v>
+      </c>
+      <c r="H30" s="2">
+        <v>272</v>
+      </c>
+      <c r="I30" s="2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="2">
+        <v>3541.138945</v>
+      </c>
+      <c r="C31" s="2">
+        <v>246.031259</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.304077</v>
+      </c>
+      <c r="E31" s="2">
+        <v>4.054082</v>
+      </c>
+      <c r="F31" s="2">
+        <v>53.125</v>
+      </c>
+      <c r="G31" s="2">
+        <v>12</v>
+      </c>
+      <c r="H31" s="2">
+        <v>272</v>
+      </c>
+      <c r="I31" s="2">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>